<commit_message>
Incorporated the new salaries into master, this is mostly all done. Just minor problems but overall its done
</commit_message>
<xml_diff>
--- a/Resources/1990/Advanced_Percentile_1990.xlsx
+++ b/Resources/1990/Advanced_Percentile_1990.xlsx
@@ -1198,43 +1198,43 @@
     <t>blabuw01</t>
   </si>
   <si>
-    <t>Karl Malone*</t>
-  </si>
-  <si>
-    <t>Michael Jordan*</t>
-  </si>
-  <si>
-    <t>Patrick Ewing*</t>
-  </si>
-  <si>
-    <t>Magic Johnson*</t>
-  </si>
-  <si>
-    <t>David Robinson*</t>
-  </si>
-  <si>
-    <t>Charles Barkley*</t>
-  </si>
-  <si>
-    <t>Chris Mullin*</t>
-  </si>
-  <si>
-    <t>Reggie Miller*</t>
-  </si>
-  <si>
-    <t>Kevin McHale*</t>
+    <t>Karl Malone</t>
+  </si>
+  <si>
+    <t>Michael Jordan</t>
+  </si>
+  <si>
+    <t>Patrick Ewing</t>
+  </si>
+  <si>
+    <t>Magic Johnson</t>
+  </si>
+  <si>
+    <t>David Robinson</t>
+  </si>
+  <si>
+    <t>Charles Barkley</t>
+  </si>
+  <si>
+    <t>Chris Mullin</t>
+  </si>
+  <si>
+    <t>Reggie Miller</t>
+  </si>
+  <si>
+    <t>Kevin McHale</t>
   </si>
   <si>
     <t>Kevin Johnson</t>
   </si>
   <si>
-    <t>Dominique Wilkins*</t>
+    <t>Dominique Wilkins</t>
   </si>
   <si>
     <t>Tom Chambers</t>
   </si>
   <si>
-    <t>Clyde Drexler*</t>
+    <t>Clyde Drexler</t>
   </si>
   <si>
     <t>Ricky Pierce</t>
@@ -1243,16 +1243,16 @@
     <t>Mark Price</t>
   </si>
   <si>
-    <t>Hakeem Olajuwon*</t>
-  </si>
-  <si>
-    <t>Larry Bird*</t>
-  </si>
-  <si>
-    <t>James Worthy*</t>
-  </si>
-  <si>
-    <t>John Stockton*</t>
+    <t>Hakeem Olajuwon</t>
+  </si>
+  <si>
+    <t>Larry Bird</t>
+  </si>
+  <si>
+    <t>James Worthy</t>
+  </si>
+  <si>
+    <t>John Stockton</t>
   </si>
   <si>
     <t>Charles Smith</t>
@@ -1270,10 +1270,10 @@
     <t>Jeff Hornacek</t>
   </si>
   <si>
-    <t>Moses Malone*</t>
-  </si>
-  <si>
-    <t>Robert Parish*</t>
+    <t>Moses Malone</t>
+  </si>
+  <si>
+    <t>Robert Parish</t>
   </si>
   <si>
     <t>Terry Cummings</t>
@@ -1288,7 +1288,7 @@
     <t>Hersey Hawkins</t>
   </si>
   <si>
-    <t>Joe Dumars*</t>
+    <t>Joe Dumars</t>
   </si>
   <si>
     <t>Orlando Woolridge</t>
@@ -1315,7 +1315,7 @@
     <t>Otis Thorpe</t>
   </si>
   <si>
-    <t>Bernard King*</t>
+    <t>Bernard King</t>
   </si>
   <si>
     <t>Derrick Gervin</t>
@@ -1339,13 +1339,13 @@
     <t>Xavier McDaniel</t>
   </si>
   <si>
-    <t>Drazen Petrovic*</t>
+    <t>Drazen Petrovic</t>
   </si>
   <si>
     <t>Mark Aguirre</t>
   </si>
   <si>
-    <t>Mitch Richmond*</t>
+    <t>Mitch Richmond</t>
   </si>
   <si>
     <t>Steve Alford</t>
@@ -1366,10 +1366,10 @@
     <t>Danny Schayes</t>
   </si>
   <si>
-    <t>Isiah Thomas*</t>
-  </si>
-  <si>
-    <t>Alex English*</t>
+    <t>Isiah Thomas</t>
+  </si>
+  <si>
+    <t>Alex English</t>
   </si>
   <si>
     <t>Armen Gilliam</t>
@@ -1390,7 +1390,7 @@
     <t>Bill Laimbeer</t>
   </si>
   <si>
-    <t>Sarunas Marciulionis*</t>
+    <t>Sarunas Marciulionis</t>
   </si>
   <si>
     <t>Charles Oakley</t>
@@ -1417,7 +1417,7 @@
     <t>Tony Campbell</t>
   </si>
   <si>
-    <t>Dennis Rodman*</t>
+    <t>Dennis Rodman</t>
   </si>
   <si>
     <t>Jerome Kersey</t>
@@ -1426,7 +1426,7 @@
     <t>Doc Rivers</t>
   </si>
   <si>
-    <t>Adrian Dantley*</t>
+    <t>Adrian Dantley</t>
   </si>
   <si>
     <t>Buck Williams</t>
@@ -1450,7 +1450,7 @@
     <t>Michael Adams</t>
   </si>
   <si>
-    <t>Scottie Pippen*</t>
+    <t>Scottie Pippen</t>
   </si>
   <si>
     <t>Michael Ansley</t>
@@ -1507,7 +1507,7 @@
     <t>Kevin Willis</t>
   </si>
   <si>
-    <t>Maurice Cheeks*</t>
+    <t>Maurice Cheeks</t>
   </si>
   <si>
     <t>Jack Sikma</t>
@@ -1861,7 +1861,7 @@
     <t>Harvey Grant</t>
   </si>
   <si>
-    <t>Dennis Johnson*</t>
+    <t>Dennis Johnson</t>
   </si>
   <si>
     <t>Steve Kerr</t>
@@ -2293,7 +2293,7 @@
     <t>Frank Kornet</t>
   </si>
   <si>
-    <t>Ralph Sampson*</t>
+    <t>Ralph Sampson</t>
   </si>
   <si>
     <t>Mike Williams</t>

</xml_diff>